<commit_message>
incorporating hyperarea calculation in features
</commit_message>
<xml_diff>
--- a/data/interim/monitor.xlsx
+++ b/data/interim/monitor.xlsx
@@ -422,13 +422,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>44469.45195979597</v>
+        <v>44469.51438932803</v>
       </c>
       <c r="C2" s="2">
-        <v>44469.45227204602</v>
+        <v>44469.51473591151</v>
       </c>
       <c r="D2" s="3">
-        <v>0.0003122500462962963</v>
+        <v>0.0003465834837962963</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -439,13 +439,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>44469.45227206592</v>
+        <v>44469.51473595767</v>
       </c>
       <c r="C3" s="2">
-        <v>44469.45253568406</v>
+        <v>44469.51505631653</v>
       </c>
       <c r="D3" s="3">
-        <v>0.0002636181481481481</v>
+        <v>0.0003203588541666667</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>